<commit_message>
Hien commit file report
</commit_message>
<xml_diff>
--- a/src/main/resources/report/BCVK-template.xlsx
+++ b/src/main/resources/report/BCVK-template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\JAVA\GIT\QLVK\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\QLVK\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5068A27-9470-458D-AEEC-974D35A27D41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>CÔNG AN TỈNH TUYÊN QUANG</t>
   </si>
@@ -76,16 +75,13 @@
     <t>Chủng loại</t>
   </si>
   <si>
-    <t>&lt;cbql&gt;</t>
-  </si>
-  <si>
-    <t>&lt;lanhdao&gt;</t>
+    <t>_cbql_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -166,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -178,6 +174,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -185,15 +190,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -225,7 +224,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -245,16 +244,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>476251</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -270,9 +269,9 @@
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="809625" y="409575"/>
-          <a:ext cx="2838450" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="2447925" y="400049"/>
+          <a:ext cx="1514476" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -300,15 +299,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -324,9 +323,9 @@
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8477250" y="409575"/>
-          <a:ext cx="2952750" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="9077325" y="390525"/>
+          <a:ext cx="2362200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -650,7 +649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -671,34 +670,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -712,61 +711,61 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="84.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -776,23 +775,23 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -835,19 +834,17 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -862,11 +859,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="A7:A8"/>
@@ -879,11 +871,16 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>